<commit_message>
feat(neverExecute): Add a new section ‘neverExecute’. If this is set to a true value a test case is not executed if this is in a reference
</commit_message>
<xml_diff>
--- a/tests/fixtures/decision/table_missing_section.xlsx
+++ b/tests/fixtures/decision/table_missing_section.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/torstenlink/Documents/entwicklung/xhubTable/file-processor/tests/fixtures/decision/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A70AC44-40CE-2049-8C3E-EEA53AF3D792}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F34D6CC-399C-0E48-A378-84606A7E9D8B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5280" yWindow="-18380" windowWidth="25060" windowHeight="13020" activeTab="1" xr2:uid="{0334C138-A09F-47F3-B471-5052FE4E750D}"/>
   </bookViews>
@@ -3845,8 +3845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0109C210-997B-2847-8039-3BFE2BEF828E}">
   <dimension ref="A1:AR72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>